<commit_message>
changed names of files
</commit_message>
<xml_diff>
--- a/weather_information.xlsx
+++ b/weather_information.xlsx
@@ -478,27 +478,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rzeszow</t>
+          <t>Legionowo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25.01℃</t>
+          <t>23.65℃</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>44/zachmurzenie</t>
+          <t>39/zachmurzenie</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>few clouds</t>
+          <t>clear sky</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1019 hPa</t>
+          <t>1018 hPa</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -511,7 +511,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2023-07-18 20:33:54</t>
+          <t>2023-07-18 20:49:17</t>
         </is>
       </c>
     </row>

</xml_diff>